<commit_message>
new changes to summary excel file
</commit_message>
<xml_diff>
--- a/Relocation Inversion Summary.xlsx
+++ b/Relocation Inversion Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/earthnote/Desktop/Bransfield/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC150B7-130B-FC4D-AD9F-D65A73443608}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC96532C-3784-844E-A7CC-3199C912D398}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10460" yWindow="460" windowWidth="17960" windowHeight="15900" xr2:uid="{183050DA-FB0A-5D41-833D-9B2202266E46}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15900" xr2:uid="{183050DA-FB0A-5D41-833D-9B2202266E46}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Station ID</t>
   </si>
@@ -107,19 +107,16 @@
     <t>BRA 27</t>
   </si>
   <si>
-    <t>Uncertainity</t>
-  </si>
-  <si>
     <t>Inverted -Bathymetry</t>
   </si>
   <si>
-    <t>station</t>
+    <t>Lon</t>
   </si>
   <si>
-    <t>Inverted Depth</t>
+    <t>Lat</t>
   </si>
   <si>
-    <t>Bathymetry Depth</t>
+    <t>Uncertainity (km)</t>
   </si>
 </sst>
 </file>
@@ -149,7 +146,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -209,11 +206,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -226,6 +260,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -233,6 +276,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -307,7 +359,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$1</c:f>
+              <c:f>Sheet1!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -317,7 +369,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -390,51 +442,51 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$3:$P$16</c:f>
+              <c:f>Sheet1!$M$3:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>2.2530656585399989E-2</c:v>
+                  <c:v>-2.0000000000000018E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-9.8863553792900571E-3</c:v>
+                  <c:v>2.0000000000000018E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3.9847345971499859E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8589003741560157E-2</c:v>
+                  <c:v>-4.0000000000000036E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-5.6065704269601113E-3</c:v>
+                  <c:v>1.0000000000000009E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-6.4030021660099745E-3</c:v>
+                  <c:v>1.0000000000000009E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3911089042998324E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.7775191509650012E-2</c:v>
+                  <c:v>2.0000000000000018E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.8037216586996094E-2</c:v>
+                  <c:v>-3.0000000000000027E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.5432256720030013E-2</c:v>
+                  <c:v>-1.0000000000000009E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.1101988886159901E-2</c:v>
+                  <c:v>-3.9999999999999813E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.9550041888726017E-2</c:v>
+                  <c:v>-4.0000000000000036E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-5.628481731219992E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-1.2275374155140018E-2</c:v>
+                  <c:v>2.0000000000000018E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -719,11 +771,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$19</c:f>
+              <c:f>Sheet1!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Inverted Depth</c:v>
+                  <c:v>z</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -752,7 +804,7 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Sheet1!$A$20:$A$33</c:f>
+              <c:f>Sheet1!$A$3:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -802,51 +854,51 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$20:$B$33</c:f>
+              <c:f>Sheet1!$I$3:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>1.4248112232646</c:v>
+                  <c:v>1.42</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5089288041592901</c:v>
+                  <c:v>1.51</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.32674065623715</c:v>
+                  <c:v>1.32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.29464439352844</c:v>
+                  <c:v>1.29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2502467162369599</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.09049482528601</c:v>
+                  <c:v>1.0900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3607778594357001</c:v>
+                  <c:v>1.36</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.1108379853096499</c:v>
+                  <c:v>1.1100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.99535827997300397</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.3409833715799699</c:v>
+                  <c:v>1.34</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1188740559838399</c:v>
+                  <c:v>1.1100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.85660452426127398</c:v>
+                  <c:v>0.85</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.41614356497122</c:v>
+                  <c:v>1.41</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.47220014656514</c:v>
+                  <c:v>1.47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -863,11 +915,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$19</c:f>
+              <c:f>Sheet1!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Bathymetry Depth</c:v>
+                  <c:v>Bathymetry Depth for inverted XY</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -896,7 +948,7 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Sheet1!$A$20:$A$33</c:f>
+              <c:f>Sheet1!$A$3:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -946,51 +998,51 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$C$33</c:f>
+              <c:f>Sheet1!$L$3:$L$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>1.44734187985</c:v>
+                  <c:v>1.44</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.49904244878</c:v>
+                  <c:v>1.49</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.32275592164</c:v>
+                  <c:v>1.32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3332333972700001</c:v>
+                  <c:v>1.33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2446401458099998</c:v>
+                  <c:v>1.24</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0840918231200001</c:v>
+                  <c:v>1.08</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3631689683399999</c:v>
+                  <c:v>1.36</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0930627937999999</c:v>
+                  <c:v>1.0900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0233954965600001</c:v>
+                  <c:v>1.02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.3564156283</c:v>
+                  <c:v>1.35</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1599760448699998</c:v>
+                  <c:v>1.1499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.89615456615</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.41051508324</c:v>
+                  <c:v>1.41</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.45992477241</c:v>
+                  <c:v>1.45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2446,16 +2498,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>598544</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>20043</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>53433</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>108313</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>982134</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>574832</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>138530</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2482,16 +2534,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>558801</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>169334</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>598072</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>125019</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>931335</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>93134</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>1456989</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>40532</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2816,64 +2868,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED6A1C9E-5628-134D-BAD5-2ADD2A0C8952}">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:C33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="94" workbookViewId="0">
+      <selection activeCell="Y41" sqref="Y41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="8" max="8" width="21.5" customWidth="1"/>
-    <col min="9" max="10" width="32.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.1640625" customWidth="1"/>
-    <col min="12" max="15" width="15.83203125" customWidth="1"/>
-    <col min="16" max="16" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" customWidth="1"/>
+    <col min="3" max="5" width="7.1640625" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" customWidth="1"/>
+    <col min="7" max="7" width="6.83203125" customWidth="1"/>
+    <col min="8" max="10" width="6.6640625" customWidth="1"/>
+    <col min="11" max="11" width="6.5" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" customWidth="1"/>
+    <col min="17" max="17" width="7" customWidth="1"/>
+    <col min="18" max="18" width="6.83203125" customWidth="1"/>
+    <col min="19" max="19" width="7" customWidth="1"/>
+    <col min="20" max="21" width="15.83203125" customWidth="1"/>
+    <col min="22" max="22" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="7"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="Q1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="10"/>
+      <c r="S1" s="11"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
+    <row r="2" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="14"/>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -2884,31 +2946,42 @@
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="2" t="s">
+      <c r="J2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="13"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -2922,44 +2995,54 @@
         <v>1.46</v>
       </c>
       <c r="E3" s="1">
+        <v>-58.599400000000003</v>
+      </c>
+      <c r="F3" s="1">
+        <v>-62.456000000000003</v>
+      </c>
+      <c r="G3" s="1">
         <v>-7.56155911368589</v>
       </c>
-      <c r="F3" s="1">
+      <c r="H3" s="1">
         <v>3.3653626842689599</v>
       </c>
-      <c r="G3" s="1">
-        <v>1.4248112232646</v>
-      </c>
-      <c r="H3" s="1">
-        <v>3.4693760912133699E-3</v>
-      </c>
       <c r="I3" s="1">
-        <v>-1447.3418798499999</v>
+        <v>1.42</v>
       </c>
       <c r="J3" s="1">
-        <f>I3*-1/1000</f>
-        <v>1.44734187985</v>
-      </c>
-      <c r="K3" s="1"/>
+        <v>-58.596853029140497</v>
+      </c>
+      <c r="K3" s="1">
+        <v>-62.456661761676202</v>
+      </c>
       <c r="L3" s="1">
-        <f>D3-G3</f>
-        <v>3.5188776735399996E-2</v>
+        <v>1.44</v>
       </c>
       <c r="M3" s="1">
-        <v>5.5723008032510304E-4</v>
+        <f t="shared" ref="M3:M16" si="0">I3-L3</f>
+        <v>-2.0000000000000018E-2</v>
       </c>
       <c r="N3" s="1">
-        <v>5.3959522859070195E-4</v>
+        <f t="shared" ref="N3:N16" si="1">I3-D3</f>
+        <v>-4.0000000000000036E-2</v>
       </c>
       <c r="O3" s="1">
-        <v>7.3671811704426504E-4</v>
+        <v>0.15</v>
       </c>
       <c r="P3" s="1">
-        <f>J3-G3</f>
-        <v>2.2530656585399989E-2</v>
+        <v>3.3999999999999998E-3</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="R3" s="1">
+        <v>5.2999999999999998E-4</v>
+      </c>
+      <c r="S3" s="1">
+        <v>7.2999999999999996E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -2973,44 +3056,54 @@
         <v>1.4950000000000001</v>
       </c>
       <c r="E4" s="1">
+        <v>-58.569899999999997</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-62.479700000000001</v>
+      </c>
+      <c r="G4" s="1">
         <v>-7.97004825637213</v>
       </c>
-      <c r="F4" s="1">
+      <c r="H4" s="1">
         <v>0.35214297181336202</v>
       </c>
-      <c r="G4" s="1">
-        <v>1.5089288041592901</v>
-      </c>
-      <c r="H4" s="1">
-        <v>4.9194221684814099E-3</v>
-      </c>
       <c r="I4" s="1">
-        <v>-1499.0424487800001</v>
+        <v>1.51</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" ref="J4:J16" si="0">I4*-1/1000</f>
-        <v>1.49904244878</v>
-      </c>
-      <c r="K4" s="1"/>
+        <v>-58.5690437638346</v>
+      </c>
+      <c r="K4" s="1">
+        <v>-62.480716962613897</v>
+      </c>
       <c r="L4" s="1">
-        <f t="shared" ref="L4:L16" si="1">D4-G4</f>
-        <v>-1.3928804159289987E-2</v>
+        <v>1.49</v>
       </c>
       <c r="M4" s="1">
-        <v>5.0591868780588197E-4</v>
+        <f t="shared" si="0"/>
+        <v>2.0000000000000018E-2</v>
       </c>
       <c r="N4" s="1">
-        <v>5.0290803658929295E-4</v>
+        <f t="shared" si="1"/>
+        <v>1.4999999999999902E-2</v>
       </c>
       <c r="O4" s="1">
-        <v>6.0160663705206298E-4</v>
+        <v>0.121</v>
       </c>
       <c r="P4" s="1">
-        <f t="shared" ref="P4:P16" si="2">J4-G4</f>
-        <v>-9.8863553792900571E-3</v>
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="R4" s="1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="S4" s="1">
+        <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -3024,44 +3117,54 @@
         <v>1.349</v>
       </c>
       <c r="E5" s="1">
+        <v>-58.548499999999997</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-62.433300000000003</v>
+      </c>
+      <c r="G5" s="1">
         <v>-3.8619484831641699</v>
       </c>
-      <c r="F5" s="1">
+      <c r="H5" s="1">
         <v>3.8600311438884298</v>
       </c>
-      <c r="G5" s="1">
-        <v>1.32674065623715</v>
-      </c>
-      <c r="H5" s="1">
-        <v>4.7883820063787802E-3</v>
-      </c>
       <c r="I5" s="1">
-        <v>-1322.75592164</v>
+        <v>1.32</v>
       </c>
       <c r="J5" s="1">
+        <v>-58.544415080519499</v>
+      </c>
+      <c r="K5" s="1">
+        <v>-62.433608924323103</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1.32</v>
+      </c>
+      <c r="M5" s="1">
         <f t="shared" si="0"/>
-        <v>1.32275592164</v>
-      </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
         <f t="shared" si="1"/>
-        <v>2.2259343762849992E-2</v>
-      </c>
-      <c r="M5" s="1">
-        <v>5.1994641073710099E-4</v>
-      </c>
-      <c r="N5" s="1">
-        <v>5.4607071704176999E-4</v>
+        <v>-2.8999999999999915E-2</v>
       </c>
       <c r="O5" s="1">
-        <v>7.9498333908233304E-4</v>
+        <v>0.21299999999999999</v>
       </c>
       <c r="P5" s="1">
-        <f t="shared" si="2"/>
-        <v>-3.9847345971499859E-3</v>
+        <v>4.7000000000000002E-3</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>5.1000000000000004E-4</v>
+      </c>
+      <c r="R5" s="1">
+        <v>5.4000000000000001E-4</v>
+      </c>
+      <c r="S5" s="1">
+        <v>7.9000000000000001E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -3075,44 +3178,54 @@
         <v>1.335</v>
       </c>
       <c r="E6" s="1">
+        <v>-58.508899999999997</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-62.454999999999998</v>
+      </c>
+      <c r="G6" s="1">
         <v>-3.70031429865098</v>
       </c>
-      <c r="F6" s="1">
+      <c r="H6" s="1">
         <v>0.70832889426908296</v>
       </c>
-      <c r="G6" s="1">
-        <v>1.29464439352844</v>
-      </c>
-      <c r="H6" s="1">
-        <v>4.2652136966582601E-3</v>
-      </c>
       <c r="I6" s="1">
-        <v>-1333.2333972700001</v>
+        <v>1.29</v>
       </c>
       <c r="J6" s="1">
+        <v>-58.506066595877201</v>
+      </c>
+      <c r="K6" s="1">
+        <v>-62.455657614820701</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1.33</v>
+      </c>
+      <c r="M6" s="1">
         <f t="shared" si="0"/>
-        <v>1.3332333972700001</v>
-      </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1">
+        <v>-4.0000000000000036E-2</v>
+      </c>
+      <c r="N6" s="1">
         <f t="shared" si="1"/>
-        <v>4.0355606471560002E-2</v>
-      </c>
-      <c r="M6" s="1">
-        <v>4.2204329808503998E-4</v>
-      </c>
-      <c r="N6" s="1">
-        <v>4.7677550023878602E-4</v>
+        <v>-4.4999999999999929E-2</v>
       </c>
       <c r="O6" s="1">
-        <v>6.3234792207162295E-4</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="P6" s="1">
-        <f t="shared" si="2"/>
-        <v>3.8589003741560157E-2</v>
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>4.2000000000000002E-4</v>
+      </c>
+      <c r="R6" s="1">
+        <v>4.6999999999999999E-4</v>
+      </c>
+      <c r="S6" s="1">
+        <v>6.3000000000000003E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -3126,44 +3239,54 @@
         <v>1.254</v>
       </c>
       <c r="E7" s="1">
+        <v>-58.494199999999999</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-62.422199999999997</v>
+      </c>
+      <c r="G7" s="1">
         <v>-0.77478342176463599</v>
       </c>
-      <c r="F7" s="1">
+      <c r="H7" s="1">
         <v>3.3264599727877</v>
       </c>
-      <c r="G7" s="1">
-        <v>1.2502467162369599</v>
-      </c>
-      <c r="H7" s="1">
-        <v>3.1986348341324299E-3</v>
-      </c>
       <c r="I7" s="1">
-        <v>-1244.6401458099999</v>
+        <v>1.25</v>
       </c>
       <c r="J7" s="1">
+        <v>-58.489968797377301</v>
+      </c>
+      <c r="K7" s="1">
+        <v>-62.421230884320401</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1.24</v>
+      </c>
+      <c r="M7" s="1">
         <f t="shared" si="0"/>
-        <v>1.2446401458099998</v>
-      </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1">
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="N7" s="1">
         <f t="shared" si="1"/>
-        <v>3.7532837630400717E-3</v>
-      </c>
-      <c r="M7" s="1">
-        <v>4.8103065090645902E-4</v>
-      </c>
-      <c r="N7" s="1">
-        <v>5.0334318796800505E-4</v>
+        <v>-4.0000000000000036E-3</v>
       </c>
       <c r="O7" s="1">
-        <v>7.7612754951112404E-4</v>
+        <v>0.24299999999999999</v>
       </c>
       <c r="P7" s="1">
-        <f t="shared" si="2"/>
-        <v>-5.6065704269601113E-3</v>
+        <v>3.0999999999999999E-3</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>4.8000000000000001E-4</v>
+      </c>
+      <c r="R7" s="1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="S7" s="1">
+        <v>7.6999999999999996E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -3177,44 +3300,54 @@
         <v>1.103</v>
       </c>
       <c r="E8" s="1">
+        <v>-58.460299999999997</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-62.4392</v>
+      </c>
+      <c r="G8" s="1">
         <v>-0.60548033371459897</v>
       </c>
-      <c r="F8" s="1">
+      <c r="H8" s="1">
         <v>0.78399193409262102</v>
       </c>
-      <c r="G8" s="1">
-        <v>1.09049482528601</v>
-      </c>
-      <c r="H8" s="1">
-        <v>4.3528991935632699E-3</v>
-      </c>
       <c r="I8" s="1">
-        <v>-1084.0918231200001</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="J8" s="1">
+        <v>-58.458408324716999</v>
+      </c>
+      <c r="K8" s="1">
+        <v>-62.438801130309599</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1.08</v>
+      </c>
+      <c r="M8" s="1">
         <f t="shared" si="0"/>
-        <v>1.0840918231200001</v>
-      </c>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1">
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="N8" s="1">
         <f t="shared" si="1"/>
-        <v>1.2505174713989931E-2</v>
-      </c>
-      <c r="M8" s="1">
-        <v>4.48817289303303E-4</v>
-      </c>
-      <c r="N8" s="1">
-        <v>4.72084272859678E-4</v>
+        <v>-1.2999999999999901E-2</v>
       </c>
       <c r="O8" s="1">
-        <v>7.2848596525978005E-4</v>
+        <v>0.107</v>
       </c>
       <c r="P8" s="1">
-        <f t="shared" si="2"/>
-        <v>-6.4030021660099745E-3</v>
+        <v>4.3E-3</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>4.4000000000000002E-4</v>
+      </c>
+      <c r="R8" s="1">
+        <v>4.6999999999999999E-4</v>
+      </c>
+      <c r="S8" s="1">
+        <v>7.2000000000000005E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3228,44 +3361,54 @@
         <v>1.3740000000000001</v>
       </c>
       <c r="E9" s="1">
+        <v>-58.454900000000002</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-62.468499999999999</v>
+      </c>
+      <c r="G9" s="1">
         <v>-2.3279376130845799</v>
       </c>
-      <c r="F9" s="1">
+      <c r="H9" s="1">
         <v>-2.0496130414351001</v>
       </c>
-      <c r="G9" s="1">
-        <v>1.3607778594357001</v>
-      </c>
-      <c r="H9" s="1">
-        <v>3.5175931649944598E-3</v>
-      </c>
       <c r="I9" s="1">
-        <v>-1363.16896834</v>
+        <v>1.36</v>
       </c>
       <c r="J9" s="1">
+        <v>-58.453153383996103</v>
+      </c>
+      <c r="K9" s="1">
+        <v>-62.468454330028997</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1.36</v>
+      </c>
+      <c r="M9" s="1">
         <f t="shared" si="0"/>
-        <v>1.3631689683399999</v>
-      </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
         <f t="shared" si="1"/>
-        <v>1.3222140564300044E-2</v>
-      </c>
-      <c r="M9" s="1">
-        <v>4.5015331929486497E-4</v>
-      </c>
-      <c r="N9" s="1">
-        <v>5.0042644631378801E-4</v>
+        <v>-1.4000000000000012E-2</v>
       </c>
       <c r="O9" s="1">
-        <v>6.6266312820310999E-4</v>
+        <v>0.09</v>
       </c>
       <c r="P9" s="1">
-        <f t="shared" si="2"/>
-        <v>2.3911089042998324E-3</v>
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>4.4999999999999999E-4</v>
+      </c>
+      <c r="R9" s="1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="S9" s="1">
+        <v>6.6E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -3279,44 +3422,54 @@
         <v>1.0920000000000001</v>
       </c>
       <c r="E10" s="1">
+        <v>-58.414000000000001</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-62.427500000000002</v>
+      </c>
+      <c r="G10" s="1">
         <v>2.0838945791921102</v>
       </c>
-      <c r="F10" s="1">
+      <c r="H10" s="1">
         <v>0.49667687233403202</v>
       </c>
-      <c r="G10" s="1">
-        <v>1.1108379853096499</v>
-      </c>
-      <c r="H10" s="1">
-        <v>5.1982148753545697E-3</v>
-      </c>
       <c r="I10" s="1">
-        <v>-1093.0627938</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="J10" s="1">
+        <v>-58.413018581621699</v>
+      </c>
+      <c r="K10" s="1">
+        <v>-62.426701925116802</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="M10" s="1">
         <f t="shared" si="0"/>
-        <v>1.0930627937999999</v>
-      </c>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1">
+        <v>2.0000000000000018E-2</v>
+      </c>
+      <c r="N10" s="1">
         <f t="shared" si="1"/>
-        <v>-1.8837985309649863E-2</v>
-      </c>
-      <c r="M10" s="1">
-        <v>4.1496906250573302E-4</v>
-      </c>
-      <c r="N10" s="1">
-        <v>4.6240689590562497E-4</v>
+        <v>1.8000000000000016E-2</v>
       </c>
       <c r="O10" s="1">
-        <v>6.9787466248758499E-4</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="P10" s="1">
-        <f t="shared" si="2"/>
-        <v>-1.7775191509650012E-2</v>
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>4.0999999999999999E-4</v>
+      </c>
+      <c r="R10" s="1">
+        <v>4.6000000000000001E-4</v>
+      </c>
+      <c r="S10" s="1">
+        <v>6.8999999999999997E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -3330,44 +3483,54 @@
         <v>1.0189999999999999</v>
       </c>
       <c r="E11" s="1">
+        <v>-58.390799999999999</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-62.436399999999999</v>
+      </c>
+      <c r="G11" s="1">
         <v>2.34930633566215</v>
       </c>
-      <c r="F11" s="1">
+      <c r="H11" s="1">
         <v>-1.05356601652086</v>
       </c>
-      <c r="G11" s="1">
-        <v>0.99535827997300397</v>
-      </c>
-      <c r="H11" s="1">
-        <v>3.9491785304573901E-3</v>
-      </c>
       <c r="I11" s="1">
-        <v>-1023.39549656</v>
+        <v>0.99</v>
       </c>
       <c r="J11" s="1">
+        <v>-58.391209156563797</v>
+      </c>
+      <c r="K11" s="1">
+        <v>-62.436549230961397</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="M11" s="1">
         <f t="shared" si="0"/>
-        <v>1.0233954965600001</v>
-      </c>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1">
+        <v>-3.0000000000000027E-2</v>
+      </c>
+      <c r="N11" s="1">
         <f t="shared" si="1"/>
-        <v>2.3641720026995938E-2</v>
-      </c>
-      <c r="M11" s="1">
-        <v>4.44626044220537E-4</v>
-      </c>
-      <c r="N11" s="1">
-        <v>5.5228725145367499E-4</v>
+        <v>-2.8999999999999915E-2</v>
       </c>
       <c r="O11" s="1">
-        <v>8.1886107577207204E-4</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="P11" s="1">
-        <f t="shared" si="2"/>
-        <v>2.8037216586996094E-2</v>
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>4.4000000000000002E-4</v>
+      </c>
+      <c r="R11" s="1">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="S11" s="1">
+        <v>8.0999999999999996E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -3381,44 +3544,54 @@
         <v>1.365</v>
       </c>
       <c r="E12" s="1">
+        <v>-58.386699999999998</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-62.463700000000003</v>
+      </c>
+      <c r="G12" s="1">
         <v>0.87663177044032004</v>
       </c>
-      <c r="F12" s="1">
+      <c r="H12" s="1">
         <v>-3.6963454330313499</v>
       </c>
-      <c r="G12" s="1">
-        <v>1.3409833715799699</v>
-      </c>
-      <c r="H12" s="1">
-        <v>3.9581879600807703E-3</v>
-      </c>
       <c r="I12" s="1">
-        <v>-1356.4156283</v>
+        <v>1.34</v>
       </c>
       <c r="J12" s="1">
+        <v>-58.384150398998798</v>
+      </c>
+      <c r="K12" s="1">
+        <v>-62.4634967261455</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1.35</v>
+      </c>
+      <c r="M12" s="1">
         <f t="shared" si="0"/>
-        <v>1.3564156283</v>
-      </c>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1">
+        <v>-1.0000000000000009E-2</v>
+      </c>
+      <c r="N12" s="1">
         <f t="shared" si="1"/>
-        <v>2.4016628420030051E-2</v>
-      </c>
-      <c r="M12" s="1">
-        <v>4.9782278131719798E-4</v>
-      </c>
-      <c r="N12" s="1">
-        <v>5.4315376866660898E-4</v>
+        <v>-2.4999999999999911E-2</v>
       </c>
       <c r="O12" s="1">
-        <v>7.9587538286582697E-4</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="P12" s="1">
-        <f t="shared" si="2"/>
-        <v>1.5432256720030013E-2</v>
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>4.8999999999999998E-4</v>
+      </c>
+      <c r="R12" s="1">
+        <v>5.4000000000000001E-4</v>
+      </c>
+      <c r="S12" s="1">
+        <v>7.9000000000000001E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
@@ -3432,44 +3605,54 @@
         <v>1.161</v>
       </c>
       <c r="E13" s="1">
+        <v>-58.400700000000001</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-62.396500000000003</v>
+      </c>
+      <c r="G13" s="1">
         <v>4.7668760402743802</v>
       </c>
-      <c r="F13" s="1">
+      <c r="H13" s="1">
         <v>2.90892126753945</v>
       </c>
-      <c r="G13" s="1">
-        <v>1.1188740559838399</v>
-      </c>
-      <c r="H13" s="1">
-        <v>6.1395311815783298E-3</v>
-      </c>
       <c r="I13" s="1">
-        <v>-1159.9760448699999</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="J13" s="1">
+        <v>-58.3984933765215</v>
+      </c>
+      <c r="K13" s="1">
+        <v>-62.395038488079699</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="M13" s="1">
         <f t="shared" si="0"/>
-        <v>1.1599760448699998</v>
-      </c>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1">
+        <v>-3.9999999999999813E-2</v>
+      </c>
+      <c r="N13" s="1">
         <f t="shared" si="1"/>
-        <v>4.21259440161601E-2</v>
-      </c>
-      <c r="M13" s="1">
-        <v>4.5979065206386602E-4</v>
-      </c>
-      <c r="N13" s="1">
-        <v>4.8150830926189502E-4</v>
+        <v>-5.0999999999999934E-2</v>
       </c>
       <c r="O13" s="1">
-        <v>8.16202456237543E-4</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="P13" s="1">
-        <f t="shared" si="2"/>
-        <v>4.1101988886159901E-2</v>
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>4.4999999999999999E-4</v>
+      </c>
+      <c r="R13" s="1">
+        <v>4.8000000000000001E-4</v>
+      </c>
+      <c r="S13" s="1">
+        <v>8.0999999999999996E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -3483,44 +3666,54 @@
         <v>1.3260000000000001</v>
       </c>
       <c r="E14" s="1">
+        <v>-58.39</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-62.414299999999997</v>
+      </c>
+      <c r="G14" s="1">
         <v>3.65116000945175</v>
       </c>
-      <c r="F14" s="1">
+      <c r="H14" s="1">
         <v>0.99014663098578404</v>
       </c>
-      <c r="G14" s="1">
-        <v>0.85660452426127398</v>
-      </c>
-      <c r="H14" s="1">
-        <v>3.2200109766894499E-3</v>
-      </c>
       <c r="I14" s="1">
-        <v>-896.15456615000005</v>
+        <v>0.85</v>
       </c>
       <c r="J14" s="1">
+        <v>-58.394108837362701</v>
+      </c>
+      <c r="K14" s="1">
+        <v>-62.414849404822</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="M14" s="1">
         <f t="shared" si="0"/>
-        <v>0.89615456615</v>
-      </c>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1">
+        <v>-4.0000000000000036E-2</v>
+      </c>
+      <c r="N14" s="1">
         <f t="shared" si="1"/>
-        <v>0.46939547573872609</v>
-      </c>
-      <c r="M14" s="1">
-        <v>4.5248464054677601E-4</v>
-      </c>
-      <c r="N14" s="1">
-        <v>4.6488456758164102E-4</v>
+        <v>-0.47600000000000009</v>
       </c>
       <c r="O14" s="1">
-        <v>1.0194775315605501E-3</v>
+        <v>0.221</v>
       </c>
       <c r="P14" s="1">
-        <f t="shared" si="2"/>
-        <v>3.9550041888726017E-2</v>
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>4.4999999999999999E-4</v>
+      </c>
+      <c r="R14" s="1">
+        <v>4.6000000000000001E-4</v>
+      </c>
+      <c r="S14" s="1">
+        <v>1E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -3534,44 +3727,54 @@
         <v>1.431</v>
       </c>
       <c r="E15" s="1">
+        <v>-58.337899999999998</v>
+      </c>
+      <c r="F15" s="1">
+        <v>-62.421300000000002</v>
+      </c>
+      <c r="G15" s="1">
         <v>5.52549478963686</v>
       </c>
-      <c r="F15" s="1">
+      <c r="H15" s="1">
         <v>-1.2369292355553101</v>
       </c>
-      <c r="G15" s="1">
-        <v>1.41614356497122</v>
-      </c>
-      <c r="H15" s="1">
-        <v>4.7391393176964601E-3</v>
-      </c>
       <c r="I15" s="1">
-        <v>-1410.51508324</v>
+        <v>1.41</v>
       </c>
       <c r="J15" s="1">
+        <v>-58.3394212217313</v>
+      </c>
+      <c r="K15" s="1">
+        <v>-62.421101711767399</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1.41</v>
+      </c>
+      <c r="M15" s="1">
         <f t="shared" si="0"/>
-        <v>1.41051508324</v>
-      </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
         <f t="shared" si="1"/>
-        <v>1.4856435028780091E-2</v>
-      </c>
-      <c r="M15" s="1">
-        <v>5.2091466628494002E-4</v>
-      </c>
-      <c r="N15" s="1">
-        <v>5.1233863791391395E-4</v>
+        <v>-2.100000000000013E-2</v>
       </c>
       <c r="O15" s="1">
-        <v>6.4124258700257598E-4</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="P15" s="1">
-        <f t="shared" si="2"/>
-        <v>-5.628481731219992E-3</v>
+        <v>4.7000000000000002E-3</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>5.1999999999999995E-4</v>
+      </c>
+      <c r="R15" s="1">
+        <v>5.1000000000000004E-4</v>
+      </c>
+      <c r="S15" s="1">
+        <v>6.4000000000000005E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -3585,250 +3788,124 @@
         <v>1.4670000000000001</v>
       </c>
       <c r="E16" s="1">
+        <v>-58.331299999999999</v>
+      </c>
+      <c r="F16" s="1">
+        <v>-62.443600000000004</v>
+      </c>
+      <c r="G16" s="1">
         <v>4.4739799106005602</v>
       </c>
-      <c r="F16" s="1">
+      <c r="H16" s="1">
         <v>-3.40458602298669</v>
       </c>
-      <c r="G16" s="1">
-        <v>1.47220014656514</v>
-      </c>
-      <c r="H16" s="1">
-        <v>7.4853794470864697E-3</v>
-      </c>
       <c r="I16" s="1">
-        <v>-1459.9247724100001</v>
+        <v>1.47</v>
       </c>
       <c r="J16" s="1">
+        <v>-58.331149747724801</v>
+      </c>
+      <c r="K16" s="1">
+        <v>-62.442375749330502</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="M16" s="1">
         <f t="shared" si="0"/>
-        <v>1.45992477241</v>
-      </c>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1">
+        <v>2.0000000000000018E-2</v>
+      </c>
+      <c r="N16" s="1">
         <f t="shared" si="1"/>
-        <v>-5.2001465651398959E-3</v>
-      </c>
-      <c r="M16" s="1">
-        <v>5.2957927873825998E-4</v>
-      </c>
-      <c r="N16" s="1">
-        <v>5.5865719998180504E-4</v>
+        <v>2.9999999999998916E-3</v>
       </c>
       <c r="O16" s="1">
-        <v>7.0836360527935696E-4</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="P16" s="1">
-        <f t="shared" si="2"/>
-        <v>-1.2275374155140018E-2</v>
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>5.1999999999999995E-4</v>
+      </c>
+      <c r="R16" s="1">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="S16" s="1">
+        <v>6.9999999999999999E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" t="s">
-        <v>28</v>
-      </c>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="1">
-        <v>1.4248112232646</v>
-      </c>
-      <c r="C20">
-        <v>1.44734187985</v>
-      </c>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="1">
-        <v>1.5089288041592901</v>
-      </c>
-      <c r="C21">
-        <v>1.49904244878</v>
-      </c>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1.32674065623715</v>
-      </c>
-      <c r="C22">
-        <v>1.32275592164</v>
-      </c>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1.29464439352844</v>
-      </c>
-      <c r="C23">
-        <v>1.3332333972700001</v>
-      </c>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="1">
-        <v>1.2502467162369599</v>
-      </c>
-      <c r="C24">
-        <v>1.2446401458099998</v>
-      </c>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="1">
-        <v>1.09049482528601</v>
-      </c>
-      <c r="C25">
-        <v>1.0840918231200001</v>
-      </c>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="1">
-        <v>1.3607778594357001</v>
-      </c>
-      <c r="C26">
-        <v>1.3631689683399999</v>
-      </c>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="1">
-        <v>1.1108379853096499</v>
-      </c>
-      <c r="C27">
-        <v>1.0930627937999999</v>
-      </c>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="1">
-        <v>0.99535827997300397</v>
-      </c>
-      <c r="C28">
-        <v>1.0233954965600001</v>
-      </c>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="1">
-        <v>1.3409833715799699</v>
-      </c>
-      <c r="C29">
-        <v>1.3564156283</v>
-      </c>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C29" s="3"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="1">
-        <v>1.1188740559838399</v>
-      </c>
-      <c r="C30">
-        <v>1.1599760448699998</v>
-      </c>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C30" s="3"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="1">
-        <v>0.85660452426127398</v>
-      </c>
-      <c r="C31">
-        <v>0.89615456615</v>
-      </c>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C31" s="3"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="1">
-        <v>1.41614356497122</v>
-      </c>
-      <c r="C32">
-        <v>1.41051508324</v>
-      </c>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C32" s="3"/>
       <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" s="1">
-        <v>1.47220014656514</v>
-      </c>
-      <c r="C33">
-        <v>1.45992477241</v>
-      </c>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C33" s="3"/>
       <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="K1:K2"/>
+  <mergeCells count="9">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="L1:L2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="I1:I2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>